<commit_message>
Fixed the Animation issue
</commit_message>
<xml_diff>
--- a/documents/Published/Rotating Chart/RotatingChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Rotating Chart/RotatingChartByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\Rotating Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srile\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E99D9-88D6-4AC9-92DA-412A9E59A37F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD40942-7ADA-442F-8667-7A8406845FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" xr2:uid="{67278F39-5C2F-4C21-84D9-7B8CB41EFB1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67278F39-5C2F-4C21-84D9-7B8CB41EFB1B}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>S no</t>
   </si>
@@ -272,6 +272,12 @@
 2. Go to 'Animation Setting' option
 3. Set toggle to ON.
 4. Update 'Delay' to 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrome </t>
+  </si>
+  <si>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -477,6 +483,511 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>140268</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5248275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3762375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16C5A324-5351-4BB6-BB65-B5FC6E627329}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11455968" y="276225"/>
+          <a:ext cx="5108007" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5286375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3438525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B074C95-DB89-4A96-8599-0AB2E868726E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11372850" y="4048124"/>
+          <a:ext cx="5229225" cy="3409951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33974</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5314950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3352800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D84364D-CA6C-4991-B1A9-D7D2B22329AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11349674" y="7562851"/>
+          <a:ext cx="5280976" cy="3305174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5333999</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3495675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D48953-16FB-41F1-8E3F-CA07D7BA08F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11344274" y="10934701"/>
+          <a:ext cx="5305425" cy="3467099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5333999</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3514725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B39F812-4ED0-4BFD-B5DB-35836AD4FDEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11344274" y="14535150"/>
+          <a:ext cx="5305425" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5010149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3781424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7763C3A9-D608-4415-BE89-708F1E4BB9A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16678274" y="238125"/>
+          <a:ext cx="4981575" cy="3733799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>16832</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5010150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3381374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D484E579-3AC1-4488-B6DA-715F84418C88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16666532" y="4038599"/>
+          <a:ext cx="4993318" cy="3362325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3371849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{637B363F-38D2-486A-BD00-9088B805E026}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16659225" y="7543799"/>
+          <a:ext cx="5086349" cy="3343275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3562350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14302E0B-C4EE-40CB-A65E-8DF4087C3FA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16659225" y="10915651"/>
+          <a:ext cx="5076824" cy="3552824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5019675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3543300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47BC3BEA-C702-4D59-A481-918ECBFD3CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16678274" y="14525625"/>
+          <a:ext cx="4991101" cy="3524250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -776,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DFE4D4-682B-4136-8526-C2C15BB103EA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,9 +1299,11 @@
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.28515625" customWidth="1"/>
+    <col min="6" max="6" width="80" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,8 +1319,14 @@
       <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="301.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -824,7 +1343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="275.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -841,7 +1360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="267" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -858,7 +1377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="283.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -875,7 +1394,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="282" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -895,6 +1414,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -902,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAF7FE4-205C-4ABB-828C-43920A88C858}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>